<commit_message>
Creación de LOG y registro de detecciones
</commit_message>
<xml_diff>
--- a/proyecto/data/info.xlsx
+++ b/proyecto/data/info.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -467,12 +467,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>LUCAS CORTES</t>
+          <t>LUCAS</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>221</t>
+          <t>lucas</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -483,10 +483,28 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n"/>
-      <c r="B3" s="1" t="n"/>
-      <c r="C3" s="1" t="n"/>
-      <c r="D3" s="1" t="n"/>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>LUCAS CORTES</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>221</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n"/>
+      <c r="B4" s="1" t="n"/>
+      <c r="C4" s="1" t="n"/>
+      <c r="D4" s="1" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Mejoramiento en la lógica de Log In y Log Out
</commit_message>
<xml_diff>
--- a/proyecto/data/info.xlsx
+++ b/proyecto/data/info.xlsx
@@ -430,37 +430,43 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col width="27.1640625" customWidth="1" min="1" max="1"/>
     <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="22.5" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Nombre</t>
+          <t>NOMBRE</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Departamento</t>
+          <t>DEPTO.</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Correo</t>
+          <t>CORREO</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Deudas</t>
+          <t>DEUDAS</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>FECHA DE MODIFICACIÓN</t>
         </is>
       </c>
     </row>
@@ -480,6 +486,11 @@
       </c>
       <c r="D2" t="n">
         <v>100000</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2020/12/09, 18:55:05</t>
+        </is>
       </c>
     </row>
     <row r="3">

</xml_diff>